<commit_message>
Update v1.4 data structure (not finish yet)
</commit_message>
<xml_diff>
--- a/SummarizeDocs/RequirementAndEstimate.xlsx
+++ b/SummarizeDocs/RequirementAndEstimate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="733" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="733" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
   <si>
     <t>List Project</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>*.jpg, *.tiff, *.txt, OCRAutoRun.exe</t>
-  </si>
-  <si>
-    <t>File name format: [OriginName]-[ID]-[1 or 2].[jpg or tiff], 0 or 1 or 2 is the number version</t>
   </si>
   <si>
     <t>File 1 line format: [ID of Rect]-;-[new ROI Rect]</t>
@@ -272,12 +269,171 @@
   <si>
     <t>File name format: [origin Image name]-Res.[jpg]</t>
   </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>tsRect</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>nID</t>
+  </si>
+  <si>
+    <t>rROI</t>
+  </si>
+  <si>
+    <t>rACVROI</t>
+  </si>
+  <si>
+    <t>strNameImage</t>
+  </si>
+  <si>
+    <t>nNumberVersion</t>
+  </si>
+  <si>
+    <t>fTimeRunning</t>
+  </si>
+  <si>
+    <t>OtherBoxes 1 element struct</t>
+  </si>
+  <si>
+    <t>Lines 1 element struct</t>
+  </si>
+  <si>
+    <t>nID;</t>
+  </si>
+  <si>
+    <t>Type    &amp;    Name</t>
+  </si>
+  <si>
+    <t>tsRect               rROI</t>
+  </si>
+  <si>
+    <t>tsRect              rACVROI</t>
+  </si>
+  <si>
+    <t>string                        strNameImage</t>
+  </si>
+  <si>
+    <t>int                            nNumberVersion</t>
+  </si>
+  <si>
+    <t>float                          fTimeRunning</t>
+  </si>
+  <si>
+    <t>int                      nID</t>
+  </si>
+  <si>
+    <t>vector&lt;pair&lt;int, tsRect&gt;&gt;               aComponentBoxes</t>
+  </si>
+  <si>
+    <t>tsBBoxInfo</t>
+  </si>
+  <si>
+    <t>teBBoxElementDataType</t>
+  </si>
+  <si>
+    <t>tsBBoxInfo, tsOtherBox</t>
+  </si>
+  <si>
+    <t>tsLineBox</t>
+  </si>
+  <si>
+    <t>BBoxIOStream</t>
+  </si>
+  <si>
+    <t>Data Structure List (class, struct, enum)</t>
+  </si>
+  <si>
+    <t>OCRAutorun</t>
+  </si>
+  <si>
+    <t>image cropped txt files</t>
+  </si>
+  <si>
+    <t>[OCR file name].txt contains all image cropped txt files</t>
+  </si>
+  <si>
+    <t>Image cropped files .jpg .png</t>
+  </si>
+  <si>
+    <t>image cropped txt files .txt</t>
+  </si>
+  <si>
+    <t>File name of 1 box in format: [OriginName]-[ID of box/rect]-[1 or 2 - Number version].[jpg or tiff], 0 or 1 or 2 is the number version</t>
+  </si>
+  <si>
+    <t>OtherBoxes.txt Number version: 0</t>
+  </si>
+  <si>
+    <t>Lines.txt Number version 0</t>
+  </si>
+  <si>
+    <t>Update OtherBoxes.txt: Number of version++</t>
+  </si>
+  <si>
+    <t>Update Lines: Number of version++</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> InputCVowel.txt</t>
+  </si>
+  <si>
+    <t>image cropped files</t>
+  </si>
+  <si>
+    <t>Get list path of image cropped txt file</t>
+  </si>
+  <si>
+    <t>Have a vowel in content ? -&gt; get ID</t>
+  </si>
+  <si>
+    <t>Get Rect</t>
+  </si>
+  <si>
+    <t>Increase Rect</t>
+  </si>
+  <si>
+    <t>Read OtherBoxes.txt and Lines.txt to find Element by ID</t>
+  </si>
+  <si>
+    <t>Run OCRAutorun</t>
+  </si>
+  <si>
+    <t>[OCR file name].txt</t>
+  </si>
+  <si>
+    <t>Check condition</t>
+  </si>
+  <si>
+    <t>VowelResult.txt</t>
+  </si>
+  <si>
+    <t>Lines.txt -&gt; Update NewROI</t>
+  </si>
+  <si>
+    <t>OtherBoxes.txt -&gt; Update NewROI</t>
+  </si>
+  <si>
+    <t>InputCVowel.txt, VowelResult.txt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +462,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,8 +560,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -634,21 +815,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="thick">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="1"/>
       </left>
@@ -667,21 +833,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -697,36 +848,8 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="medium">
         <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color theme="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
@@ -955,11 +1078,219 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1030,56 +1361,76 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1089,49 +1440,87 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1451,7 +1840,7 @@
       <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="57" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1465,7 +1854,7 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:4" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -1477,7 +1866,7 @@
       <c r="C4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="1:4" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
@@ -1489,7 +1878,7 @@
       <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -1501,7 +1890,7 @@
       <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="51"/>
+      <c r="D6" s="59"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1515,34 +1904,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="97.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="32"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -1554,386 +1940,454 @@
       <c r="D2" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="26" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39">
+        <v>1</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
+        <v>2</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="177" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
+        <v>3</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="215.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="39">
         <v>4</v>
       </c>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27">
+      <c r="B6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="C6" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
+        <v>5</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="32"/>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="27">
+      <c r="C7" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="39">
+        <v>6</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>7</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
+        <v>8</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="39">
+        <v>9</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
+        <v>10</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>11</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>12</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>13</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>14</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="44">
+        <v>15</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:4" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
+    </row>
+    <row r="21" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="69"/>
+      <c r="B21" s="70"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="71"/>
+    </row>
+    <row r="22" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="72"/>
+      <c r="B22" s="73"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="74"/>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="47"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+    </row>
+    <row r="24" spans="1:4" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+    </row>
+    <row r="25" spans="1:4" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="26"/>
+      <c r="B25" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <v>1</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="32"/>
-    </row>
-    <row r="5" spans="1:6" ht="165.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="27">
+      <c r="B27" s="32"/>
+      <c r="C27" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="32"/>
-    </row>
-    <row r="6" spans="1:6" ht="186.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27">
+      <c r="B28" s="35"/>
+      <c r="C28" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="32"/>
-    </row>
-    <row r="7" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
+      <c r="B29" s="35"/>
+      <c r="C29" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="28"/>
-      <c r="F7" s="32"/>
-    </row>
-    <row r="8" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
-        <v>6</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="32"/>
-    </row>
-    <row r="9" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
-        <v>7</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="32"/>
-    </row>
-    <row r="10" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <v>8</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="32"/>
-    </row>
-    <row r="11" spans="1:6" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27">
-        <v>9</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="32"/>
-    </row>
-    <row r="12" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
-        <v>10</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="32"/>
-    </row>
-    <row r="13" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27">
-        <v>11</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="32"/>
-    </row>
-    <row r="14" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27">
-        <v>12</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="32"/>
-    </row>
-    <row r="15" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27">
-        <v>13</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="32"/>
-    </row>
-    <row r="16" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
-        <v>14</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="32"/>
-    </row>
-    <row r="17" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="64">
-        <v>15</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="30" t="s">
+      <c r="B30" s="36"/>
+      <c r="C30" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="47"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+    </row>
+    <row r="32" spans="1:4" ht="24" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="61"/>
+      <c r="D32" s="48" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-    </row>
-    <row r="18" spans="1:6" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:6" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-    </row>
-    <row r="21" spans="1:6" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="57"/>
-    </row>
-    <row r="22" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="58"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="60"/>
-    </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="61"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="63"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:6" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-    </row>
-    <row r="27" spans="1:6" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="37"/>
-      <c r="B27" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E27" s="37"/>
-    </row>
-    <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36">
-        <v>1</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="36"/>
-    </row>
-    <row r="29" spans="1:6" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="36">
-        <v>2</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="36"/>
-    </row>
-    <row r="30" spans="1:6" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="36">
-        <v>3</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="36"/>
-    </row>
-    <row r="31" spans="1:6" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="36">
-        <v>4</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="42"/>
-      <c r="E31" s="36"/>
-    </row>
-    <row r="32" spans="1:6" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="36">
-        <v>5</v>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="36"/>
-    </row>
-    <row r="33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C33" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="62"/>
+      <c r="B35" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="62"/>
+      <c r="B36" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="62"/>
+      <c r="B37" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="62"/>
+      <c r="B38" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="62"/>
+      <c r="B39" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A21:E23"/>
+  <mergeCells count="6">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A20:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1944,7 +2398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -1956,26 +2410,292 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="42.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="76"/>
+    </row>
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="55">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="55">
+        <v>2</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="55">
+        <v>3</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="55">
+        <v>4</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="55">
+        <v>5</v>
+      </c>
+      <c r="B6" s="55"/>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="55">
+        <v>6</v>
+      </c>
+      <c r="B7" s="55"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="56">
+        <v>7</v>
+      </c>
+      <c r="B8" s="56"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="83"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="83"/>
+    </row>
+    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="81"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="83"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="84"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="86"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A4:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="19.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="79" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="82"/>
+      <c r="C5" s="79" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="83" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="81"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="83"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="81"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="83"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="86"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update complete OCRAutoRun module
</commit_message>
<xml_diff>
--- a/SummarizeDocs/RequirementAndEstimate.xlsx
+++ b/SummarizeDocs/RequirementAndEstimate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="733" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" tabRatio="733" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
   <si>
     <t>List Project</t>
   </si>
@@ -234,9 +234,6 @@
 &lt;/Rect&gt;</t>
   </si>
   <si>
-    <t>Input Image -&gt; General Control -&gt; OCRAutoRun(OCR boxes after MSER and filter) -&gt; CheckVowel(check if result contains vowels) -&gt; OCRAutoRun(OCR boxes which have vowels) -&gt; MergeTextToImage(handle old and new result after OCR) -&gt; Lexicon -&gt; MergeTextToImage (add text to image) -&gt; Output Image</t>
-  </si>
-  <si>
     <t>Folder</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>int                      nID</t>
   </si>
   <si>
-    <t>vector&lt;pair&lt;int, tsRect&gt;&gt;               aComponentBoxes</t>
-  </si>
-  <si>
     <t>tsBBoxInfo</t>
   </si>
   <si>
@@ -427,6 +421,59 @@
   </si>
   <si>
     <t>InputCVowel.txt, VowelResult.txt</t>
+  </si>
+  <si>
+    <t>vector&lt;int&gt; SubID</t>
+  </si>
+  <si>
+    <t>vector&lt;tsRect&gt; subRect</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Having input image</t>
+  </si>
+  <si>
+    <t>Stored in TmpImage</t>
+  </si>
+  <si>
+    <t>GeneralControl</t>
+  </si>
+  <si>
+    <t>txt files are stored in TmpRect, jpg files are stored in TmpImage</t>
+  </si>
+  <si>
+    <t>Format Input/Output</t>
+  </si>
+  <si>
+    <t>Output: .jpg</t>
+  </si>
+  <si>
+    <t>Input: *.jpg, Files.txt
+Output: OtherBoxes.txt, Lines.txt, *.jpg</t>
+  </si>
+  <si>
+    <t>Input: *OtherBoxes.txt, Lines.txt, *.jpg
+Output: *.jpg, *.txt (output from tesseract), InputCVowel.txt</t>
+  </si>
+  <si>
+    <t>*.txt and *.jpg files are stored in TmpImage.
+InputCVowel.txt is stored in TmpCheckVowel.</t>
+  </si>
+  <si>
+    <t>Input: InputCVowel.txt, OtherBoxes.txt, Lines.txt, *.jpg
+Output: nothing or [modify OtherBoxes.txt, Lines.txt, new *.jpg]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Image -&gt; General Control -&gt; OCRAutoRun(OCR boxes after MSER and filter) -&gt; CheckVowel(check if result contains vowels) -&gt; OCRAutoRun(OCR boxes which have vowels) -&gt; MergeTextToImage(handle old and new result after OCR) -&gt; Lexicon -&gt; MergeTextToImage (add text to image) -&gt; Output Image
+CheckVowel increase Rect format:
+&lt; 10pixel: increase 2
+else height: 15%, width: 2
+</t>
   </si>
 </sst>
 </file>
@@ -573,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -1286,11 +1333,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashDot">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="dashDot">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="dashDot">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1410,9 +1631,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1431,6 +1649,88 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1440,6 +1740,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1455,9 +1758,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1490,36 +1790,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1840,7 +2110,7 @@
       <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="86" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1854,7 +2124,7 @@
       <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="58"/>
+      <c r="D3" s="87"/>
     </row>
     <row r="4" spans="1:4" ht="86.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
@@ -1866,7 +2136,7 @@
       <c r="C4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="87"/>
     </row>
     <row r="5" spans="1:4" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
@@ -1878,7 +2148,7 @@
       <c r="C5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="87"/>
     </row>
     <row r="6" spans="1:4" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
@@ -1890,7 +2160,7 @@
       <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="59"/>
+      <c r="D6" s="88"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1904,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1920,12 +2190,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -2008,7 +2278,7 @@
         <v>30</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2103,10 +2373,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2117,10 +2387,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="43" t="s">
         <v>63</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2131,10 +2401,10 @@
         <v>8</v>
       </c>
       <c r="C16" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="43" t="s">
         <v>65</v>
-      </c>
-      <c r="D16" s="43" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2145,10 +2415,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2158,32 +2428,32 @@
       <c r="D18" s="24"/>
     </row>
     <row r="19" spans="1:4" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="89"/>
+      <c r="D19" s="89"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
+      <c r="A20" s="95" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="96"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
     </row>
     <row r="21" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="70"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="71"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="100"/>
     </row>
     <row r="22" spans="1:4" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="72"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
+      <c r="A22" s="101"/>
+      <c r="B22" s="102"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="103"/>
     </row>
     <row r="23" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="47"/>
@@ -2192,23 +2462,23 @@
       <c r="D23" s="47"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="B24" s="89"/>
+      <c r="C24" s="89"/>
+      <c r="D24" s="89"/>
     </row>
     <row r="25" spans="1:4" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="26"/>
       <c r="B25" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="D25" s="27" t="s">
         <v>59</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2256,7 +2526,7 @@
         <v>50</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2278,110 +2548,229 @@
       <c r="D31" s="47"/>
     </row>
     <row r="32" spans="1:4" ht="24" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="60" t="s">
+      <c r="B32" s="90" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="91"/>
+      <c r="D32" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="48" t="s">
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="52" t="s">
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="92"/>
+      <c r="B35" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="92"/>
+      <c r="B36" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="92"/>
+      <c r="B37" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="92"/>
+      <c r="B38" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="62"/>
-      <c r="B35" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="B36" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="62"/>
-      <c r="B37" s="49" t="s">
+      <c r="C38" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="92"/>
+      <c r="B39" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" s="49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="62"/>
-      <c r="B38" s="49" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="49" t="s">
+      <c r="C39" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D39" s="52" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="62"/>
-      <c r="B39" s="50" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="D39" s="53" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="68"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:7" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="89"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="73" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="69">
+        <v>1</v>
+      </c>
+      <c r="B45" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="75">
+        <v>2</v>
+      </c>
+      <c r="B46" s="76" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="77" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="78">
+        <v>3</v>
+      </c>
+      <c r="B47" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="80" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="82">
+        <v>4</v>
+      </c>
+      <c r="B48" s="80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="81"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="82">
+        <v>5</v>
+      </c>
+      <c r="B49" s="80"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="81"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="82">
+        <v>6</v>
+      </c>
+      <c r="B50" s="80"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="81"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="82">
+        <v>7</v>
+      </c>
+      <c r="B51" s="80"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="81"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="83">
+        <v>8</v>
+      </c>
+      <c r="B52" s="84"/>
+      <c r="C52" s="84"/>
+      <c r="D52" s="85"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A43:D43"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="A34:A39"/>
     <mergeCell ref="A1:D1"/>
@@ -2426,127 +2815,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="76"/>
+      <c r="A1" s="104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="105"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="55">
+      <c r="A2" s="54">
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="54">
+        <v>2</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="54">
+        <v>3</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="55">
-        <v>2</v>
-      </c>
-      <c r="B3" s="55" t="s">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="54">
+        <v>4</v>
+      </c>
+      <c r="B5" s="54" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="55">
-        <v>3</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="55">
-        <v>4</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="55">
+      <c r="A6" s="54">
         <v>5</v>
       </c>
-      <c r="B6" s="55"/>
+      <c r="B6" s="54"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="55">
+      <c r="A7" s="54">
         <v>6</v>
       </c>
-      <c r="B7" s="55"/>
+      <c r="B7" s="54"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="56">
+      <c r="A8" s="55">
         <v>7</v>
       </c>
-      <c r="B8" s="56"/>
+      <c r="B8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="62"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="62"/>
+    </row>
+    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="60"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="79" t="s">
-        <v>106</v>
-      </c>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="81" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="82"/>
-      <c r="D12" s="82" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="83"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="81" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="83"/>
-    </row>
-    <row r="14" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="83"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="84"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="85"/>
-      <c r="I15" s="86"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2561,7 +2950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -2582,118 +2971,118 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="77" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="61"/>
+      <c r="C5" s="58" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79" t="s">
+      <c r="F5" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="I5" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="80" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="79" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="82" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="82" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="82" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="83" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="83" t="s">
-        <v>120</v>
-      </c>
-    </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="83"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="83"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="86"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>